<commit_message>
Coorect legal_addr & delivery_type
</commit_message>
<xml_diff>
--- a/appl_register.xlsx
+++ b/appl_register.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="110">
   <si>
     <t>Менеджер</t>
   </si>
@@ -79,10 +79,19 @@
     <t>\nЗаявка на самовывоз \n1. Дата отгрузки: \n28.04.2024 \nЦем I 42,5Н/ Кричев \n3. Количество машин/тонн: 70 тонн \n4. Перевалка Сзтк \n5.Покупатель груза: "ЗАО ПК ТЕРМОБЕТОН  \n6. Продажа от ООО «СЗТК»\n\nн223вм977 Музафяров Руслан\n</t>
   </si>
   <si>
+    <t>\nАлексей Мельхер:\nЗаявка на доставку \n1.Дата отгрузки 28.04\n2. Марка: ЦЕМ I 42.5Н Костюковичи \n3. Количество: 70 тонн     \n4. Продажа от ООО "СЗТК" \n5. С Солнечногорска \n6. Покупатель ООО «М Бетон» \n7. Грузополучатель ООО «М-Бетон» \n8. Юр.Адрес грузополучателя: 109382, г. Москва, вн. тер. г. муниципальный округ Люблино, ул. Люблинская, д. 72, помещ. 26 \n9. Пункт разгрузки: Москва г, Очаковское ш., дом 5А, въезд с проезда Стройкомбината\n10. Контакты для связи 8-925-758-01-54\n</t>
+  </si>
+  <si>
+    <t>\nЗаявка на доставку  \n1. Дата отгрузки:  29.04\n2. Марка цемента: ЦЕМ I 42,5 Н Кричев/Костюковичи\n3. Кол-во 140 тонн\n4. Продажа от клиента: ООО Спарта    \n5. Завод отгрузки: КПП, Солнечногорск, Люберцы \n6. Покупатель груза: ООО «Сибирский элемент Рента - К»    \n7. Грузополучателя (при оформлении ТТН): ООО «Сибирский элемент Рента - К»    \n8. Адрес грузополучателя (юрид): 249850, Калужская обл., Дзержинский р-н, д. Обуховской, д 1Б.    \n9. Пункт разгрузки (факт): Калужская обл., Дзержинский р-н, д. Обухово 1Б    \n10. Плательщик транспортировки (при оформлении ТТН):    \nКонтактный телефон 8 (965) 709-90-77 Игорь.\nПриёмка круглосуточно\n</t>
+  </si>
+  <si>
     <t>доставка</t>
   </si>
   <si>
     <t>самовывоз</t>
+  </si>
+  <si>
+    <t>автономка доставка</t>
   </si>
   <si>
     <t>26.04.2024</t>
@@ -340,8 +349,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,22 +409,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -453,7 +457,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -487,7 +491,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -522,10 +525,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -698,16 +700,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,920 +760,1169 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F2">
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="M2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="N2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="P2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="Q2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F3">
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="N3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F4">
         <v>120</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F5">
         <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="N5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="O5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F6">
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F7">
         <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="L7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="L8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F9">
         <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F10">
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M10" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="N10" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="O10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F11">
         <v>120</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F12">
         <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I12" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="N12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F13">
         <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I13" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F14">
         <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J14" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N14" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O14" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="Q14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F15">
         <v>200</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I15" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="L15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="N15" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="O15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="P15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F16">
         <v>200</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I16" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="L16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="N16" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="O16" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="P16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F17">
         <v>105</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J17" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="N17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F18">
         <v>140</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I18" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J18" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K18" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="M18" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="N18" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O18" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="P18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F19">
         <v>40</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J19" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="K19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="N19" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O19" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="P19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F20">
         <v>70</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I20" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J20" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="K20" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M20" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N20" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F21">
         <v>40</v>
       </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K21" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L21" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="N21" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="B22" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F22">
         <v>70</v>
       </c>
       <c r="G22" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H22" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I22" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J22" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="B23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F23">
         <v>70</v>
       </c>
       <c r="G23" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H23" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I23" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J23" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="B24" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F24">
         <v>70</v>
       </c>
       <c r="G24" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H24" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I24" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J24" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F25">
         <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I25" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J25" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K25" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L25" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="N25" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F26">
         <v>40</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I26" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J26" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K26" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L26" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="N26" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28">
+        <v>35</v>
+      </c>
+      <c r="G28" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" t="s">
+        <v>75</v>
+      </c>
+      <c r="L28" t="s">
+        <v>75</v>
+      </c>
+      <c r="N28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29">
+        <v>35</v>
+      </c>
+      <c r="G29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" t="s">
+        <v>65</v>
+      </c>
+      <c r="K29" t="s">
+        <v>75</v>
+      </c>
+      <c r="L29" t="s">
+        <v>75</v>
+      </c>
+      <c r="N29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33">
+        <v>140</v>
+      </c>
+      <c r="G33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" t="s">
+        <v>60</v>
+      </c>
+      <c r="J33" t="s">
+        <v>70</v>
+      </c>
+      <c r="K33" t="s">
+        <v>80</v>
+      </c>
+      <c r="M33" t="s">
+        <v>90</v>
+      </c>
+      <c r="N33" t="s">
+        <v>92</v>
+      </c>
+      <c r="O33" t="s">
+        <v>100</v>
+      </c>
+      <c r="P33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34">
+        <v>70</v>
+      </c>
+      <c r="G34" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" t="s">
+        <v>61</v>
+      </c>
+      <c r="J34" t="s">
+        <v>72</v>
+      </c>
+      <c r="K34" t="s">
+        <v>82</v>
+      </c>
+      <c r="L34" t="s">
+        <v>86</v>
+      </c>
+      <c r="M34" t="s">
+        <v>91</v>
+      </c>
+      <c r="N34" t="s">
+        <v>92</v>
+      </c>
+      <c r="O34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35">
+        <v>35</v>
+      </c>
+      <c r="G35" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" t="s">
+        <v>55</v>
+      </c>
+      <c r="J35" t="s">
+        <v>65</v>
+      </c>
+      <c r="K35" t="s">
+        <v>75</v>
+      </c>
+      <c r="L35" t="s">
+        <v>75</v>
+      </c>
+      <c r="N35" t="s">
+        <v>93</v>
+      </c>
+      <c r="O35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36">
+        <v>40</v>
+      </c>
+      <c r="G36" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" t="s">
+        <v>55</v>
+      </c>
+      <c r="J36" t="s">
+        <v>71</v>
+      </c>
+      <c r="K36" t="s">
+        <v>81</v>
+      </c>
+      <c r="L36" t="s">
+        <v>81</v>
+      </c>
+      <c r="N36" t="s">
+        <v>92</v>
+      </c>
+      <c r="O36" t="s">
+        <v>101</v>
+      </c>
+      <c r="P36" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added product & product notice as methods
</commit_message>
<xml_diff>
--- a/appl_register.xlsx
+++ b/appl_register.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="ошибки" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="115">
   <si>
     <t>Менеджер</t>
   </si>
@@ -67,6 +68,9 @@
     <t>Примечание Иное</t>
   </si>
   <si>
+    <t>Текст заявки</t>
+  </si>
+  <si>
     <t>Игорь Хабаров</t>
   </si>
   <si>
@@ -344,6 +348,18 @@
   </si>
   <si>
     <t>оплата 250</t>
+  </si>
+  <si>
+    <t>\nИГО:\nЗаявка на доставку \n1. Дата отгрузки 28.04.2023 \n2. Марка ЦЕМ I 42.5н Беларусь   \n3. Количество 40 тонн  \n4. От ООО Спарта \n5. Завод: Сзтк \n6. Покупатель ООО ""ТД"Цемент \n7. Грузополучатель: ООО "ТД"Цемент  \n8. Голицыно\n+7 910 404-06-14\nРБУ\nМожайское ш., 81\n</t>
+  </si>
+  <si>
+    <t>\nЮра Менеджер:\nЗаявка на доставку (автономка) \n1. Дата отгрузки: 28.04.24 \n2. Марка: ЦЕМ I 42,5н БЦЗ Костюковичи \nМашина с пломбами и актуальными паспортами \n3. Количество: 40т.\n4. Продажа от: ООО "Спарта"\n5. Перевалка: СЗТК \n6. Покупатель: ООО "КАНТАН"\n7. Грузополучатель: ООО "КАНТАН"\n8. Время приёмки: к 9 \n9. Контакт диспетчера: +79777728931 \n10. Точка выгрузки: территориальное управление Соколовское\nгородской округ Солнечногорск, Московская область\n</t>
+  </si>
+  <si>
+    <t>Ошибка</t>
+  </si>
+  <si>
+    <t>Заявка</t>
   </si>
 </sst>
 </file>
@@ -701,13 +717,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -759,1170 +775,1243 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F2">
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="P2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F3">
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F4">
         <v>120</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5">
         <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6">
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7">
         <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F8">
         <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F9">
         <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F10">
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F11">
         <v>120</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F12">
         <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F13">
         <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F14">
         <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F15">
         <v>200</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F16">
         <v>200</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F17">
         <v>105</v>
       </c>
       <c r="G17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F18">
         <v>140</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F19">
         <v>40</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F20">
         <v>70</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F21">
         <v>40</v>
       </c>
       <c r="G21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="B22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F22">
         <v>70</v>
       </c>
       <c r="G22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="B23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F23">
         <v>70</v>
       </c>
       <c r="G23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="B24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F24">
         <v>70</v>
       </c>
       <c r="G24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F25">
         <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N25" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F26">
         <v>40</v>
       </c>
       <c r="G26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L26" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N26" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O26" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:16">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F28">
         <v>35</v>
       </c>
       <c r="G28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J28" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F29">
         <v>35</v>
       </c>
       <c r="G29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:16">
       <c r="A32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F33">
         <v>140</v>
       </c>
       <c r="G33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N33" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O33" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P33" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F34">
         <v>70</v>
       </c>
       <c r="G34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K34" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L34" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N34" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O34" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F35">
         <v>35</v>
       </c>
       <c r="G35" t="s">
+        <v>49</v>
+      </c>
+      <c r="I35" t="s">
+        <v>56</v>
+      </c>
+      <c r="J35" t="s">
+        <v>66</v>
+      </c>
+      <c r="K35" t="s">
+        <v>76</v>
+      </c>
+      <c r="L35" t="s">
+        <v>76</v>
+      </c>
+      <c r="N35" t="s">
+        <v>94</v>
+      </c>
+      <c r="O35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" t="s">
         <v>48</v>
-      </c>
-      <c r="I35" t="s">
-        <v>55</v>
-      </c>
-      <c r="J35" t="s">
-        <v>65</v>
-      </c>
-      <c r="K35" t="s">
-        <v>75</v>
-      </c>
-      <c r="L35" t="s">
-        <v>75</v>
-      </c>
-      <c r="N35" t="s">
-        <v>93</v>
-      </c>
-      <c r="O35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
-      <c r="A36" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" t="s">
-        <v>47</v>
       </c>
       <c r="F36">
         <v>40</v>
       </c>
       <c r="G36" t="s">
+        <v>49</v>
+      </c>
+      <c r="I36" t="s">
+        <v>56</v>
+      </c>
+      <c r="J36" t="s">
+        <v>72</v>
+      </c>
+      <c r="K36" t="s">
+        <v>82</v>
+      </c>
+      <c r="L36" t="s">
+        <v>82</v>
+      </c>
+      <c r="N36" t="s">
+        <v>93</v>
+      </c>
+      <c r="O36" t="s">
+        <v>102</v>
+      </c>
+      <c r="P36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37">
+        <v>40</v>
+      </c>
+      <c r="G37" t="s">
+        <v>49</v>
+      </c>
+      <c r="K37" t="s">
+        <v>84</v>
+      </c>
+      <c r="R37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" t="s">
         <v>48</v>
       </c>
-      <c r="I36" t="s">
-        <v>55</v>
-      </c>
-      <c r="J36" t="s">
-        <v>71</v>
-      </c>
-      <c r="K36" t="s">
-        <v>81</v>
-      </c>
-      <c r="L36" t="s">
-        <v>81</v>
-      </c>
-      <c r="N36" t="s">
-        <v>92</v>
-      </c>
-      <c r="O36" t="s">
-        <v>101</v>
-      </c>
-      <c r="P36" t="s">
-        <v>108</v>
+      <c r="F38">
+        <v>40</v>
+      </c>
+      <c r="G38" t="s">
+        <v>49</v>
+      </c>
+      <c r="K38" t="s">
+        <v>82</v>
+      </c>
+      <c r="R38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added dates extracting method
</commit_message>
<xml_diff>
--- a/appl_register.xlsx
+++ b/appl_register.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="121">
   <si>
     <t>Менеджер</t>
   </si>
@@ -354,6 +354,24 @@
   </si>
   <si>
     <t>\nЮра Менеджер:\nЗаявка на доставку (автономка) \n1. Дата отгрузки: 28.04.24 \n2. Марка: ЦЕМ I 42,5н БЦЗ Костюковичи \nМашина с пломбами и актуальными паспортами \n3. Количество: 40т.\n4. Продажа от: ООО "Спарта"\n5. Перевалка: СЗТК \n6. Покупатель: ООО "КАНТАН"\n7. Грузополучатель: ООО "КАНТАН"\n8. Время приёмки: к 9 \n9. Контакт диспетчера: +79777728931 \n10. Точка выгрузки: территориальное управление Соколовское\nгородской округ Солнечногорск, Московская область\n</t>
+  </si>
+  <si>
+    <t>\nИГО:\nЗаявка на доставку \n1. Дата отгрузки 28.04.2024 \n2. Марка ЦЕМ I 42.5н Беларусь   \n3. Количество 40 тонн  \n4. От ООО Спарта \n5. Завод: Сзтк \n6. Покупатель ООО ""ТД"Цемент \n7. Грузополучатель: ООО "ТД"Цемент  \n8. Голицыно\n+7 910 404-06-14\nРБУ\nМожайское ш., 81\n</t>
+  </si>
+  <si>
+    <t>\nЮра Менеджер:\n1. Дата отгрузки:\n26.04.2024\n2. От ООО Спарта\n3. Марка: Щебень гранитный 5-20(ЛСР)\nОбязательно актуальный паспорт!\n4. Покупатель ООО НВЛ ГРУП\n5. Бетас \n6.  Количество 120т\n7. Машина: \nО327ВН790 МАN\nО039ОУ790 МАN,\nХ194ВА797 КАМАЗ\nВ683СН790 МАN\nМ991ХС750 МАN\nО030ХЕ123 МАN\nВ551ВО790 МАN\nС289УТ750 МАN\nВ247ХО750 МАN \nУ162ХК750 MAN\nХ240ВА797 КАМАЗ\n А215УХ750 МAN\n</t>
+  </si>
+  <si>
+    <t>\nИГО:\n1. Дата отгрузки\n26.04.2024\n2.Марка цемента ЦЕМ I 42.5Н БЦК \n3. Количество 35 тонн \n4. Продажа от ООО "Спарта"\n5. С псо 13\n6. Покупатель ООО "Бетонная индустрия»\n7. Грузополучатель ООО "Бетонная индустрия»\n8. Адрес грузополучателя \nОдинцово \nКобяковская. Краснознаменск.\n</t>
+  </si>
+  <si>
+    <t>\nИГО:\n1. Дата отгрузки\n26.4.2024\n2.Марка цемента ЦЕМ I 42.5Н БЦК \n3. Количество 35 тонн \n4. Продажа от ООО "Спарта"\n5. С псо 13\n6. Покупатель ООО "Бетонная индустрия»\n7. Грузополучатель ООО "Бетонная индустрия»\n8. Адрес грузополучателя \nОдинцово \nКобяковская. Краснознаменск.\n</t>
+  </si>
+  <si>
+    <t>ИГО:1. Дата отгрузки26.04.20242.Марка цемента ЦЕМ I 42.5Н БЦК 3. Количество 35 тонн 4. Продажа от ООО "Спарта"5. С псо 136. Покупатель ООО "Бетонная индустрия»7. Грузополучатель ООО "Бетонная индустрия»8. Адрес грузополучателя Одинцово Кобяковская. Краснознаменск.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ИГО: 1. Дата отгрузки 26.04.2024 2.Марка цемента ЦЕМ I 42.5Н БЦК  3. Количество 35 тонн  4. Продажа от ООО "Спарта" 5. С псо 13 6. Покупатель ООО "Бетонная индустрия» 7. Грузополучатель ООО "Бетонная индустрия» 8. Адрес грузополучателя  Одинцово  Кобяковская. Краснознаменск. </t>
   </si>
   <si>
     <t>Ошибка</t>
@@ -717,7 +735,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R38"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1991,6 +2009,203 @@
       </c>
       <c r="R38" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="R39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="R40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="R41" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42" t="s">
+        <v>49</v>
+      </c>
+      <c r="K42" t="s">
+        <v>84</v>
+      </c>
+      <c r="R42" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43">
+        <v>120</v>
+      </c>
+      <c r="G43" t="s">
+        <v>49</v>
+      </c>
+      <c r="K43" t="s">
+        <v>77</v>
+      </c>
+      <c r="R43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44">
+        <v>35</v>
+      </c>
+      <c r="G44" t="s">
+        <v>49</v>
+      </c>
+      <c r="K44" t="s">
+        <v>76</v>
+      </c>
+      <c r="R44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45">
+        <v>35</v>
+      </c>
+      <c r="G45" t="s">
+        <v>49</v>
+      </c>
+      <c r="K45" t="s">
+        <v>76</v>
+      </c>
+      <c r="R45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46">
+        <v>35</v>
+      </c>
+      <c r="G46" t="s">
+        <v>49</v>
+      </c>
+      <c r="K46" t="s">
+        <v>76</v>
+      </c>
+      <c r="R46" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47">
+        <v>35</v>
+      </c>
+      <c r="G47" t="s">
+        <v>49</v>
+      </c>
+      <c r="K47" t="s">
+        <v>76</v>
+      </c>
+      <c r="R47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48">
+        <v>35</v>
+      </c>
+      <c r="G48" t="s">
+        <v>49</v>
+      </c>
+      <c r="K48" t="s">
+        <v>76</v>
+      </c>
+      <c r="R48" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2008,10 +2223,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added organization, transshipment, purchaser
</commit_message>
<xml_diff>
--- a/appl_register.xlsx
+++ b/appl_register.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="123">
   <si>
     <t>Менеджер</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t xml:space="preserve"> ИГО: 1. Дата отгрузки 26.04.2024 2.Марка цемента ЦЕМ I 42.5Н БЦК  3. Количество 35 тонн  4. Продажа от ООО "Спарта" 5. С псо 13 6. Покупатель ООО "Бетонная индустрия» 7. Грузополучатель ООО "Бетонная индустрия» 8. Адрес грузополучателя  Одинцово  Кобяковская. Краснознаменск. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Заявка на самовывоз  1. Дата отгрузки:  28.04.2024  Марка Цем I 42,5Н/ Кричев  3. Количество машин/тонн: 70 тонн  4. Перевалка Сзтк  5.Покупатель груза: "ЗАО ПК ТЕРМОБЕТОН   6. Продажа от ООО «СЗТК»  н223вм977 Музафяров Руслан н095вм977 Трушев Давид Т132ак977 Бабий Антон Т132Ак977 Савинец Юрий Н223ВМ977 Маркин Александр Н095ВМ977 Шаркевич Алексей </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Юра Менеджер: Заявка/ самовывоз 1. Дата отгрузки: 26.04.24 2. Марка цемента: ЦЕМ I 42.5Н БЦЗ Костюковичи  3. Кол-во машин/ тонн: 100т 4. Продажа от клиента: ОО0 Спарта  5. Завод отгрузки: СЗТК 6. Покупатель груза:ООО "Форма ЖБИ" 7. Грузополучатель (при оформлении ттн): ООО "Форма ЖбИ" 8. М192МС90</t>
   </si>
   <si>
     <t>Ошибка</t>
@@ -735,7 +741,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2206,6 +2212,119 @@
       </c>
       <c r="R48" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49">
+        <v>70</v>
+      </c>
+      <c r="G49" t="s">
+        <v>49</v>
+      </c>
+      <c r="H49" t="s">
+        <v>55</v>
+      </c>
+      <c r="K49" t="s">
+        <v>85</v>
+      </c>
+      <c r="R49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" t="s">
+        <v>37</v>
+      </c>
+      <c r="F50">
+        <v>100</v>
+      </c>
+      <c r="G50" t="s">
+        <v>49</v>
+      </c>
+      <c r="K50" t="s">
+        <v>78</v>
+      </c>
+      <c r="R50" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" t="s">
+        <v>37</v>
+      </c>
+      <c r="F51">
+        <v>100</v>
+      </c>
+      <c r="G51" t="s">
+        <v>49</v>
+      </c>
+      <c r="I51" t="s">
+        <v>59</v>
+      </c>
+      <c r="K51" t="s">
+        <v>78</v>
+      </c>
+      <c r="R51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" t="s">
+        <v>37</v>
+      </c>
+      <c r="F52">
+        <v>100</v>
+      </c>
+      <c r="G52" t="s">
+        <v>49</v>
+      </c>
+      <c r="I52" t="s">
+        <v>59</v>
+      </c>
+      <c r="J52" t="s">
+        <v>68</v>
+      </c>
+      <c r="K52" t="s">
+        <v>78</v>
+      </c>
+      <c r="R52" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2223,10 +2342,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the rest methods
</commit_message>
<xml_diff>
--- a/appl_register.xlsx
+++ b/appl_register.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="ошибки" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="130">
   <si>
     <t>Менеджер</t>
   </si>
@@ -53,7 +53,7 @@
     <t>Грузополучатель</t>
   </si>
   <si>
-    <t>Адрес грузополучателя (юрид)</t>
+    <t>Юр. адрес грузополучателя</t>
   </si>
   <si>
     <t>Адрес пункта разгрузки</t>
@@ -155,6 +155,9 @@
     <t xml:space="preserve">Цем I 42,5Н/ Кричев </t>
   </si>
   <si>
+    <t>: ЦЕМ I 42,5 Н Кричев/Костюковичи</t>
+  </si>
+  <si>
     <t>Сертификаты!</t>
   </si>
   <si>
@@ -284,6 +287,9 @@
     <t>ООО "ТД"Цемент</t>
   </si>
   <si>
+    <t>ООО «Сибирский элемент Рента - К»</t>
+  </si>
+  <si>
     <t xml:space="preserve">249850, Калужская обл., Дзержинский р-н, д. Обуховской, д 1Б. </t>
   </si>
   <si>
@@ -350,6 +356,9 @@
     <t>оплата 250</t>
   </si>
   <si>
+    <t>Оплата мильён</t>
+  </si>
+  <si>
     <t>\nИГО:\nЗаявка на доставку \n1. Дата отгрузки 28.04.2023 \n2. Марка ЦЕМ I 42.5н Беларусь   \n3. Количество 40 тонн  \n4. От ООО Спарта \n5. Завод: Сзтк \n6. Покупатель ООО ""ТД"Цемент \n7. Грузополучатель: ООО "ТД"Цемент  \n8. Голицыно\n+7 910 404-06-14\nРБУ\nМожайское ш., 81\n</t>
   </si>
   <si>
@@ -378,6 +387,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Юра Менеджер: Заявка/ самовывоз 1. Дата отгрузки: 26.04.24 2. Марка цемента: ЦЕМ I 42.5Н БЦЗ Костюковичи  3. Кол-во машин/ тонн: 100т 4. Продажа от клиента: ОО0 Спарта  5. Завод отгрузки: СЗТК 6. Покупатель груза:ООО "Форма ЖБИ" 7. Грузополучатель (при оформлении ттн): ООО "Форма ЖбИ" 8. М192МС90</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Заявка на доставку   1. Дата отгрузки:  29.04 2. Марка цемента: ЦЕМ I 42,5 Н Кричев/Костюковичи 3. Кол-во 140 тонн 4. Продажа от клиента: ООО Спарта     5. Завод отгрузки: КПП, Солнечногорск, Люберцы  6. Покупатель груза: ООО «Сибирский элемент Рента - К»     7. Грузополучателя (при оформлении ТТН): ООО «Сибирский элемент Рента - К»     8. Адрес грузополучателя (юрид): 249850, Калужская обл., Дзержинский р-н, д. Обуховской, д 1Б.     9. Пункт разгрузки (факт): Калужская обл., Дзержинский р-н, д. Обухово 1Б     10. Плательщик транспортировки (при оформлении ТТН):     Контактный телефон 8 (965) 709-90-77 Игорь. Приёмка круглосуточно </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Заявка на доставку   1. Дата отгрузки:  29.04 2. Марка цемента: ЦЕМ I 42,5 Н Кричев/Костюковичи 3. Кол-во 140 тонн 4. Продажа от клиента: ООО Спарта     5. Завод отгрузки: КПП, Солнечногорск, Люберцы  6. Покупатель груза: ООО «Сибирский элемент Рента - К»     7. Грузополучатель (при оформлении ТТН): ООО «Сибирский элемент Рента - К»     8. Адрес грузополучателя (юрид): 249850, Калужская обл., Дзержинский р-н, д. Обуховской, д 1Б.     9. Пункт разгрузки (факт): Калужская обл., Дзержинский р-н, д. Обухово 1Б     10. Плательщик транспортировки (при оформлении ТТН):     Контактный телефон 8 (965) 709-90-77 Игорь. Приёмка круглосуточно </t>
+  </si>
+  <si>
+    <t>\nЗаявка на доставку  \n1. Дата отгрузки:  29.04\n2. Марка цемента: ЦЕМ I 42,5 Н Кричев/Костюковичи\n3. Кол-во 140 тонн\n4. Продажа от клиента: ООО Спарта    \n5. Завод отгрузки: КПП, Солнечногорск, Люберцы \n6. Покупатель груза: ООО «Сибирский элемент Рента - К»    \n7. Грузополучателя (при оформлении ТТН): ООО «Сибирский элемент Рента - К»    \n8. Адрес грузополучателя (юрид): 249850, Калужская обл., Дзержинский р-н, д. Обуховской, д 1Б.    \n9. Пункт разгрузки (факт): Калужская обл., Дзержинский р-н, д. Обухово 1Б    \n10. Плательщик транспортировки (при оформлении ТТН): \n Оплата мильён   \nКонтактный телефон 8 (965) 709-90-77 Игорь.\nПриёмка круглосуточно\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Заявка на доставку   1. Дата отгрузки:  29.04 2. Марка цемента: ЦЕМ I 42,5 Н Кричев/Костюковичи 3. Кол-во 140 тонн 4. Продажа от клиента: ООО Спарта     5. Завод отгрузки: КПП, Солнечногорск, Люберцы  6. Покупатель груза: ООО «Сибирский элемент Рента - К»     7. Грузополучателя (при оформлении ТТН): ООО «Сибирский элемент Рента - К»     8. Адрес грузополучателя (юрид): 249850, Калужская обл., Дзержинский р-н, д. Обуховской, д 1Б.     9. Пункт разгрузки (факт): Калужская обл., Дзержинский р-н, д. Обухово 1Б     10. Плательщик транспортировки (при оформлении ТТН):   Оплата мильён    Контактный телефон 8 (965) 709-90-77 Игорь. Приёмка круглосуточно </t>
   </si>
   <si>
     <t>Ошибка</t>
@@ -389,8 +410,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,17 +470,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -497,7 +523,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -531,6 +557,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -565,9 +592,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -740,14 +768,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="Q65" sqref="Q65"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,7 +833,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -817,46 +847,46 @@
         <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2">
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="N2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="O2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="P2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -873,28 +903,28 @@
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -908,25 +938,25 @@
         <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F4">
         <v>120</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -943,31 +973,31 @@
         <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -984,19 +1014,19 @@
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1013,22 +1043,22 @@
         <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1045,22 +1075,22 @@
         <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1077,19 +1107,19 @@
         <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1106,31 +1136,31 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1144,25 +1174,25 @@
         <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F11">
         <v>120</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1179,28 +1209,28 @@
         <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1217,19 +1247,19 @@
         <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1246,31 +1276,31 @@
         <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="O14" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="Q14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1287,31 +1317,31 @@
         <v>200</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="P15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1328,31 +1358,31 @@
         <v>200</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="P16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1369,25 +1399,25 @@
         <v>105</v>
       </c>
       <c r="G17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1404,31 +1434,31 @@
         <v>140</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M18" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="N18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="O18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1442,37 +1472,37 @@
         <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F19">
         <v>40</v>
       </c>
       <c r="G19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="O19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="P19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1489,31 +1519,31 @@
         <v>70</v>
       </c>
       <c r="G20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M20" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="N20" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="O20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1530,28 +1560,28 @@
         <v>40</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I21" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N21" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="O21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>25</v>
       </c>
@@ -1565,22 +1595,22 @@
         <v>70</v>
       </c>
       <c r="G22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>25</v>
       </c>
@@ -1594,22 +1624,22 @@
         <v>70</v>
       </c>
       <c r="G23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>25</v>
       </c>
@@ -1623,22 +1653,22 @@
         <v>70</v>
       </c>
       <c r="G24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1655,28 +1685,28 @@
         <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K25" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="O25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -1693,33 +1723,33 @@
         <v>40</v>
       </c>
       <c r="G26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N26" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="O26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1736,25 +1766,25 @@
         <v>35</v>
       </c>
       <c r="G28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J28" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1771,40 +1801,40 @@
         <v>35</v>
       </c>
       <c r="G29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -1821,31 +1851,31 @@
         <v>140</v>
       </c>
       <c r="G33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I33" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M33" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="N33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="O33" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1862,31 +1892,31 @@
         <v>70</v>
       </c>
       <c r="G34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I34" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L34" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M34" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="N34" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="O34" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1903,28 +1933,28 @@
         <v>35</v>
       </c>
       <c r="G35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I35" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J35" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N35" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O35" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -1938,37 +1968,37 @@
         <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F36">
         <v>40</v>
       </c>
       <c r="G36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I36" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J36" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N36" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="O36" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="P36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -1982,16 +2012,16 @@
         <v>40</v>
       </c>
       <c r="G37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="R37" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -2002,37 +2032,37 @@
         <v>42</v>
       </c>
       <c r="E38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F38">
         <v>40</v>
       </c>
       <c r="G38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K38" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R38" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R39" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R40" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="R41" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -2049,16 +2079,16 @@
         <v>40</v>
       </c>
       <c r="G42" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="R42" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -2072,22 +2102,22 @@
         <v>35</v>
       </c>
       <c r="E43" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F43">
         <v>120</v>
       </c>
       <c r="G43" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K43" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="R43" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -2104,16 +2134,16 @@
         <v>35</v>
       </c>
       <c r="G44" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K44" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R44" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -2127,16 +2157,16 @@
         <v>35</v>
       </c>
       <c r="G45" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R45" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -2153,16 +2183,16 @@
         <v>35</v>
       </c>
       <c r="G46" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K46" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R46" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2179,16 +2209,16 @@
         <v>35</v>
       </c>
       <c r="G47" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K47" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R47" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -2205,16 +2235,16 @@
         <v>35</v>
       </c>
       <c r="G48" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K48" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R48" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>25</v>
       </c>
@@ -2228,19 +2258,19 @@
         <v>70</v>
       </c>
       <c r="G49" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H49" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K49" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="R49" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -2257,16 +2287,16 @@
         <v>100</v>
       </c>
       <c r="G50" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="R50" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -2283,19 +2313,19 @@
         <v>100</v>
       </c>
       <c r="G51" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I51" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K51" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="R51" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -2312,19 +2342,420 @@
         <v>100</v>
       </c>
       <c r="G52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K52" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="R52" t="s">
-        <v>120</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" t="s">
+        <v>37</v>
+      </c>
+      <c r="F53">
+        <v>100</v>
+      </c>
+      <c r="G53" t="s">
+        <v>50</v>
+      </c>
+      <c r="I53" t="s">
+        <v>60</v>
+      </c>
+      <c r="J53" t="s">
+        <v>69</v>
+      </c>
+      <c r="K53" t="s">
+        <v>79</v>
+      </c>
+      <c r="L53" t="s">
+        <v>87</v>
+      </c>
+      <c r="R53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" t="s">
+        <v>46</v>
+      </c>
+      <c r="F55">
+        <v>140</v>
+      </c>
+      <c r="G55" t="s">
+        <v>50</v>
+      </c>
+      <c r="I55" t="s">
+        <v>62</v>
+      </c>
+      <c r="J55" t="s">
+        <v>72</v>
+      </c>
+      <c r="K55" t="s">
+        <v>82</v>
+      </c>
+      <c r="M55" t="s">
+        <v>93</v>
+      </c>
+      <c r="R55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57">
+        <v>140</v>
+      </c>
+      <c r="G57" t="s">
+        <v>50</v>
+      </c>
+      <c r="I57" t="s">
+        <v>62</v>
+      </c>
+      <c r="J57" t="s">
+        <v>72</v>
+      </c>
+      <c r="K57" t="s">
+        <v>82</v>
+      </c>
+      <c r="M57" t="s">
+        <v>93</v>
+      </c>
+      <c r="O57" t="s">
+        <v>103</v>
+      </c>
+      <c r="R57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R58" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59" t="s">
+        <v>46</v>
+      </c>
+      <c r="F59">
+        <v>140</v>
+      </c>
+      <c r="G59" t="s">
+        <v>50</v>
+      </c>
+      <c r="I59" t="s">
+        <v>62</v>
+      </c>
+      <c r="J59" t="s">
+        <v>72</v>
+      </c>
+      <c r="K59" t="s">
+        <v>82</v>
+      </c>
+      <c r="M59" t="s">
+        <v>93</v>
+      </c>
+      <c r="N59" t="s">
+        <v>95</v>
+      </c>
+      <c r="O59" t="s">
+        <v>103</v>
+      </c>
+      <c r="R59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" t="s">
+        <v>46</v>
+      </c>
+      <c r="F60">
+        <v>140</v>
+      </c>
+      <c r="G60" t="s">
+        <v>50</v>
+      </c>
+      <c r="I60" t="s">
+        <v>62</v>
+      </c>
+      <c r="J60" t="s">
+        <v>72</v>
+      </c>
+      <c r="K60" t="s">
+        <v>82</v>
+      </c>
+      <c r="L60" t="s">
+        <v>90</v>
+      </c>
+      <c r="M60" t="s">
+        <v>93</v>
+      </c>
+      <c r="N60" t="s">
+        <v>95</v>
+      </c>
+      <c r="O60" t="s">
+        <v>103</v>
+      </c>
+      <c r="R60" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" t="s">
+        <v>46</v>
+      </c>
+      <c r="F61">
+        <v>140</v>
+      </c>
+      <c r="G61" t="s">
+        <v>50</v>
+      </c>
+      <c r="I61" t="s">
+        <v>62</v>
+      </c>
+      <c r="J61" t="s">
+        <v>72</v>
+      </c>
+      <c r="K61" t="s">
+        <v>82</v>
+      </c>
+      <c r="L61" t="s">
+        <v>90</v>
+      </c>
+      <c r="M61" t="s">
+        <v>93</v>
+      </c>
+      <c r="N61" t="s">
+        <v>95</v>
+      </c>
+      <c r="O61" t="s">
+        <v>103</v>
+      </c>
+      <c r="R61" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62" t="s">
+        <v>46</v>
+      </c>
+      <c r="F62">
+        <v>140</v>
+      </c>
+      <c r="G62" t="s">
+        <v>50</v>
+      </c>
+      <c r="I62" t="s">
+        <v>62</v>
+      </c>
+      <c r="J62" t="s">
+        <v>72</v>
+      </c>
+      <c r="K62" t="s">
+        <v>82</v>
+      </c>
+      <c r="L62" t="s">
+        <v>90</v>
+      </c>
+      <c r="M62" t="s">
+        <v>93</v>
+      </c>
+      <c r="N62" t="s">
+        <v>95</v>
+      </c>
+      <c r="O62" t="s">
+        <v>103</v>
+      </c>
+      <c r="P62" t="s">
+        <v>110</v>
+      </c>
+      <c r="R62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64" t="s">
+        <v>46</v>
+      </c>
+      <c r="F64">
+        <v>140</v>
+      </c>
+      <c r="G64" t="s">
+        <v>50</v>
+      </c>
+      <c r="I64" t="s">
+        <v>62</v>
+      </c>
+      <c r="J64" t="s">
+        <v>72</v>
+      </c>
+      <c r="K64" t="s">
+        <v>82</v>
+      </c>
+      <c r="L64" t="s">
+        <v>90</v>
+      </c>
+      <c r="M64" t="s">
+        <v>93</v>
+      </c>
+      <c r="N64" t="s">
+        <v>95</v>
+      </c>
+      <c r="O64" t="s">
+        <v>103</v>
+      </c>
+      <c r="P64" t="s">
+        <v>110</v>
+      </c>
+      <c r="R64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" t="s">
+        <v>30</v>
+      </c>
+      <c r="D65" t="s">
+        <v>46</v>
+      </c>
+      <c r="F65">
+        <v>140</v>
+      </c>
+      <c r="G65" t="s">
+        <v>50</v>
+      </c>
+      <c r="I65" t="s">
+        <v>62</v>
+      </c>
+      <c r="J65" t="s">
+        <v>72</v>
+      </c>
+      <c r="K65" t="s">
+        <v>82</v>
+      </c>
+      <c r="L65" t="s">
+        <v>90</v>
+      </c>
+      <c r="M65" t="s">
+        <v>93</v>
+      </c>
+      <c r="N65" t="s">
+        <v>95</v>
+      </c>
+      <c r="O65" t="s">
+        <v>103</v>
+      </c>
+      <c r="P65" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>113</v>
+      </c>
+      <c r="R65" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2333,19 +2764,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added error handling decorator
</commit_message>
<xml_diff>
--- a/appl_register.xlsx
+++ b/appl_register.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="ошибки" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="81">
   <si>
     <t>№ Заявки</t>
   </si>
@@ -98,6 +98,9 @@
     <t>28.04.2024</t>
   </si>
   <si>
+    <t>28.04.2023</t>
+  </si>
+  <si>
     <t>ПЕСКОГРУНТ</t>
   </si>
   <si>
@@ -113,6 +116,9 @@
     <t>Щебень гранитный 5-20(ЛСР)</t>
   </si>
   <si>
+    <t xml:space="preserve">ЦЕМ I 42.5н Беларусь   </t>
+  </si>
+  <si>
     <t>Обязательно актуальный паспорт!</t>
   </si>
   <si>
@@ -128,6 +134,9 @@
     <t>О327ВН790 МАN, О039ОУ790 МАN, Х194ВА797 КАМАЗ, В683СН790 МАN, М991ХС750 МАN, О030ХЕ123 МАN, В551ВО790 МАN, С289УТ750 МАN, В247ХО750 МАN, У162ХК750 MAN, Х240ВА797 КАМАЗ, А215УХ750 МAN</t>
   </si>
   <si>
+    <t>н223вм977 Музафяров, н095вм977 Трушев, Т132ак977 Бабий, Т132Ак977 Савинец, Н223ВМ977 Маркин, Н095ВМ977 Шаркевич</t>
+  </si>
+  <si>
     <t>ООО "Спарта"</t>
   </si>
   <si>
@@ -137,6 +146,9 @@
     <t>ООО Спарта</t>
   </si>
   <si>
+    <t xml:space="preserve">ООО Спарта </t>
+  </si>
+  <si>
     <t>🤷\u200d♂️</t>
   </si>
   <si>
@@ -164,6 +176,12 @@
     <t>ООО НВЛ ГРУП</t>
   </si>
   <si>
+    <t xml:space="preserve">ООО ""ТД"Цемент </t>
+  </si>
+  <si>
+    <t>ООО "ТД"Цемент</t>
+  </si>
+  <si>
     <t>Москва, Бескудниковский бульвар, 52к1</t>
   </si>
   <si>
@@ -173,12 +191,18 @@
     <t>Одинцово. Кобяковская. Краснознаменск.</t>
   </si>
   <si>
+    <t>Голицыно, Можайское ш., 81, РБУ</t>
+  </si>
+  <si>
     <t>+7 968 558-83-13</t>
   </si>
   <si>
     <t>+79232208000, +74959242828</t>
   </si>
   <si>
+    <t>+7 910 404-06-14</t>
+  </si>
+  <si>
     <t>с 9.00 до 20.00</t>
   </si>
   <si>
@@ -207,6 +231,27 @@
   </si>
   <si>
     <t xml:space="preserve"> Юра Менеджер: 1. Дата отгрузки: 26.04.2024 2. От ООО Спарта 3. Марка: Щебень гранитный 5-20(ЛСР) Обязательно актуальный паспорт! 4. Покупатель ООО НВЛ ГРУП 5. Бетас  6.  Количество 105 кубов  7. Машина:  О327ВН790 МАN О039ОУ790 МАN, Х194ВА797 КАМАЗ В683СН790 МАN М991ХС750 МАN О030ХЕ123 МАN В551ВО790 МАN С289УТ750 МАN В247ХО750 МАN  У162ХК750 MAN Х240ВА797 КАМАЗ  А215УХ750 МAN </t>
+  </si>
+  <si>
+    <t>\nИГО:\n1. Дата отгрузки\n25.04.2024\n2.Марка цемента ЦЕМ I 42.5Н БЦК \n3. Количество 35 тонн \n4. Продажа от ООО "Спарта"\n5. С псо 13\n6. Покупатель ООО "Бетонная индустрия»\n7. Грузополучатель ООО "Бетонная индустрия»\n8. Адрес грузополучателя \nОдинцово \nКобяковская. Краснознаменск. \n8 (903) 007-00-86\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Заявка на самовывоз  1. Дата отгрузки:  28.04.2024  Марка Цем I 42,5Н/ Кричев  3. Количество машин/тонн: 70 тонн  4. Перевалка Сзтк  5.Покупатель груза: "ЗАО ПК ТЕРМОБЕТОН   6. Продажа от ООО «СЗТК»  н223вм977 Музафяров Руслан н095вм977 Трушев Давид Т132ак977 Бабий Антон Т132Ак977 Савинец Юрий Н223ВМ977 Маркин Александр Н095ВМ977 Шаркевич Алексей </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ИГО: Заявка на доставку  1. Дата отгрузки 28.04.2023  2. Марка ЦЕМ I 42.5н Беларусь    3. Количество 40 тонн   4. От ООО Спарта  5. Завод: Сзтк  6. Покупатель ООО ""ТД"Цемент  7. Грузополучатель: ООО "ТД"Цемент   8. Голицыно +7 910 404-06-14 РБУ Можайское ш., 81 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ИГО: Заявка на доставку  1. Дата отгрузки 28.04.2023  2. Марка ЦЕМ I 42.5н Беларусь    3. Количество тонн: 40   4. От ООО Спарта  5. Завод: Сзтк  6. Покупатель ООО ""ТД"Цемент  7. Грузополучатель: ООО "ТД"Цемент   8. Голицыно +7 910 404-06-14 РБУ Можайское ш., 81 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ИГО: Заявка на доставку  1. Дата отгрузки 28.04.2023  2. Марка ЦЕМ I 42.5н Беларусь    3. Количество тонн: 140   4. От ООО Спарта  5. Завод: Сзтк  6. Покупатель ООО ""ТД"Цемент  7. Грузополучатель: ООО "ТД"Цемент   8. Голицыно +7 910 404-06-14 РБУ Можайское ш., 81 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Заявка на доставку  1. Дата отгрузки 28.04.2023  2. Марка ЦЕМ I 42.5н Беларусь    3. Количество тонн: 200   4. От ООО Спарта  5. Завод: Сзтк  6. Покупатель ООО ""ТД"Цемент  7. Грузополучатель: ООО "ТД"Цемент   8. Голицыно +7 910 404-06-14 РБУ Можайское ш., 81 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ИГО:  Заявка на доставку  1. Дата отгрузки 28.04.2023  2. Марка ЦЕМ I 42.5н Беларусь    3. Количество тонн: 200   4. От ООО Спарта  5. Завод: Сзтк  6. Покупатель ООО ""ТД"Цемент  7. Грузополучатель: ООО "ТД"Цемент   8. Голицыно +7 910 404-06-14 РБУ Можайское ш., 81 </t>
   </si>
   <si>
     <t>Ошибка</t>
@@ -218,8 +263,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,17 +323,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -326,7 +376,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -360,6 +410,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -394,9 +445,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -569,14 +621,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +689,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -649,40 +703,40 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G2">
         <v>200</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="P2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -696,40 +750,40 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3">
         <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="O3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="P3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="R3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="S3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -743,40 +797,40 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G4">
         <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="O4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="P4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="R4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="S4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -790,40 +844,40 @@
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5">
         <v>80</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="O5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="P5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="R5" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="S5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -837,40 +891,40 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>80</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="O6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="P6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="R6" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="S6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -884,40 +938,40 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="O7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="P7" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="R7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="S7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -931,40 +985,40 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G8">
         <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="O8" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="P8" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="R8" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="S8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -978,40 +1032,40 @@
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G9">
         <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="O9" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="P9" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="R9" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="S9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1025,40 +1079,40 @@
         <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>40</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="P10" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q10" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1072,40 +1126,40 @@
         <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G11">
         <v>40</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O11" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="P11" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q11" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1119,40 +1173,40 @@
         <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G12">
         <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L12" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M12" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O12" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="P12" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q12" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1166,40 +1220,40 @@
         <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G13">
         <v>40</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K13" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O13" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="P13" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1213,40 +1267,40 @@
         <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G14">
         <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K14" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O14" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="P14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q14" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1260,40 +1314,40 @@
         <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G15">
         <v>40</v>
       </c>
       <c r="H15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O15" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="P15" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q15" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1307,40 +1361,40 @@
         <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G16">
         <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K16" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L16" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M16" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O16" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="P16" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q16" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1354,40 +1408,40 @@
         <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G17">
         <v>40</v>
       </c>
       <c r="H17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J17" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K17" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O17" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="P17" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q17" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1401,40 +1455,40 @@
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G18">
         <v>40</v>
       </c>
       <c r="H18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J18" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K18" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L18" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M18" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O18" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="P18" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q18" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1448,48 +1502,48 @@
         <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G19">
         <v>40</v>
       </c>
       <c r="H19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J19" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K19" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L19" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M19" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O19" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="P19" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q19" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="S20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1500,31 +1554,31 @@
         <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G21">
         <v>40</v>
       </c>
       <c r="H21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J21" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K21" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="L21" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="S21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1535,31 +1589,31 @@
         <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G22">
         <v>40</v>
       </c>
       <c r="H22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I22" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K22" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="L22" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="S22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1570,31 +1624,31 @@
         <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G23">
         <v>40</v>
       </c>
       <c r="H23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J23" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="L23" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="S23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1608,34 +1662,34 @@
         <v>25</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G24">
         <v>40</v>
       </c>
       <c r="H24" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J24" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K24" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L24" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M24" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O24" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="S24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1649,34 +1703,34 @@
         <v>25</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G25">
         <v>40</v>
       </c>
       <c r="H25" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J25" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K25" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L25" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M25" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O25" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="S25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1690,31 +1744,31 @@
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F26" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G26">
         <v>40</v>
       </c>
       <c r="H26" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J26" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L26" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="S26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1728,31 +1782,31 @@
         <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G27">
         <v>40</v>
       </c>
       <c r="H27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J27" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L27" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="S27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1766,28 +1820,955 @@
         <v>25</v>
       </c>
       <c r="E28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28">
+        <v>40</v>
+      </c>
+      <c r="H28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" t="s">
+        <v>38</v>
+      </c>
+      <c r="J28" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" t="s">
+        <v>52</v>
+      </c>
+      <c r="S28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="S29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30">
+        <v>35</v>
+      </c>
+      <c r="H30" t="s">
+        <v>36</v>
+      </c>
+      <c r="I30" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" t="s">
+        <v>41</v>
+      </c>
+      <c r="K30" t="s">
+        <v>46</v>
+      </c>
+      <c r="L30" t="s">
+        <v>50</v>
+      </c>
+      <c r="S30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31">
+        <v>35</v>
+      </c>
+      <c r="H31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31" t="s">
+        <v>41</v>
+      </c>
+      <c r="K31" t="s">
+        <v>46</v>
+      </c>
+      <c r="L31" t="s">
+        <v>50</v>
+      </c>
+      <c r="S31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="F28" t="s">
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32">
+        <v>35</v>
+      </c>
+      <c r="H32" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32" t="s">
+        <v>43</v>
+      </c>
+      <c r="K32" t="s">
+        <v>46</v>
+      </c>
+      <c r="L32" t="s">
+        <v>53</v>
+      </c>
+      <c r="M32" t="s">
+        <v>54</v>
+      </c>
+      <c r="O32" t="s">
+        <v>58</v>
+      </c>
+      <c r="P32" t="s">
+        <v>61</v>
+      </c>
+      <c r="S32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="G28">
-        <v>40</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" t="s">
         <v>33</v>
       </c>
-      <c r="I28" t="s">
+      <c r="G33">
+        <v>40</v>
+      </c>
+      <c r="J33" t="s">
+        <v>43</v>
+      </c>
+      <c r="K33" t="s">
+        <v>46</v>
+      </c>
+      <c r="L33" t="s">
+        <v>53</v>
+      </c>
+      <c r="M33" t="s">
+        <v>54</v>
+      </c>
+      <c r="O33" t="s">
+        <v>58</v>
+      </c>
+      <c r="P33" t="s">
+        <v>61</v>
+      </c>
+      <c r="S33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34">
+        <v>40</v>
+      </c>
+      <c r="J34" t="s">
+        <v>43</v>
+      </c>
+      <c r="K34" t="s">
+        <v>46</v>
+      </c>
+      <c r="L34" t="s">
+        <v>53</v>
+      </c>
+      <c r="M34" t="s">
+        <v>54</v>
+      </c>
+      <c r="O34" t="s">
+        <v>58</v>
+      </c>
+      <c r="P34" t="s">
+        <v>61</v>
+      </c>
+      <c r="S34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35">
+        <v>40</v>
+      </c>
+      <c r="J35" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" t="s">
+        <v>46</v>
+      </c>
+      <c r="L35" t="s">
+        <v>53</v>
+      </c>
+      <c r="M35" t="s">
+        <v>54</v>
+      </c>
+      <c r="O35" t="s">
+        <v>58</v>
+      </c>
+      <c r="P35" t="s">
+        <v>61</v>
+      </c>
+      <c r="S35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" t="s">
+        <v>33</v>
+      </c>
+      <c r="G36">
+        <v>40</v>
+      </c>
+      <c r="J36" t="s">
+        <v>43</v>
+      </c>
+      <c r="K36" t="s">
+        <v>46</v>
+      </c>
+      <c r="L36" t="s">
+        <v>53</v>
+      </c>
+      <c r="M36" t="s">
+        <v>54</v>
+      </c>
+      <c r="O36" t="s">
+        <v>58</v>
+      </c>
+      <c r="P36" t="s">
+        <v>61</v>
+      </c>
+      <c r="S36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="J28" t="s">
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
+      <c r="G37">
+        <v>40</v>
+      </c>
+      <c r="J37" t="s">
+        <v>43</v>
+      </c>
+      <c r="K37" t="s">
+        <v>46</v>
+      </c>
+      <c r="L37" t="s">
+        <v>53</v>
+      </c>
+      <c r="M37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O37" t="s">
+        <v>58</v>
+      </c>
+      <c r="P37" t="s">
+        <v>61</v>
+      </c>
+      <c r="S37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+      <c r="G38">
+        <v>40</v>
+      </c>
+      <c r="J38" t="s">
+        <v>43</v>
+      </c>
+      <c r="K38" t="s">
+        <v>46</v>
+      </c>
+      <c r="L38" t="s">
+        <v>53</v>
+      </c>
+      <c r="M38" t="s">
+        <v>54</v>
+      </c>
+      <c r="O38" t="s">
+        <v>58</v>
+      </c>
+      <c r="P38" t="s">
+        <v>61</v>
+      </c>
+      <c r="S38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G39">
+        <v>40</v>
+      </c>
+      <c r="J39" t="s">
+        <v>43</v>
+      </c>
+      <c r="K39" t="s">
+        <v>46</v>
+      </c>
+      <c r="L39" t="s">
+        <v>53</v>
+      </c>
+      <c r="M39" t="s">
+        <v>54</v>
+      </c>
+      <c r="O39" t="s">
+        <v>58</v>
+      </c>
+      <c r="P39" t="s">
+        <v>61</v>
+      </c>
+      <c r="S39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="L28" t="s">
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G40">
+        <v>40</v>
+      </c>
+      <c r="J40" t="s">
+        <v>43</v>
+      </c>
+      <c r="K40" t="s">
+        <v>46</v>
+      </c>
+      <c r="L40" t="s">
+        <v>53</v>
+      </c>
+      <c r="M40" t="s">
+        <v>54</v>
+      </c>
+      <c r="O40" t="s">
+        <v>58</v>
+      </c>
+      <c r="P40" t="s">
+        <v>61</v>
+      </c>
+      <c r="S40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41">
+        <v>40</v>
+      </c>
+      <c r="J41" t="s">
+        <v>43</v>
+      </c>
+      <c r="K41" t="s">
+        <v>46</v>
+      </c>
+      <c r="L41" t="s">
+        <v>53</v>
+      </c>
+      <c r="M41" t="s">
+        <v>54</v>
+      </c>
+      <c r="O41" t="s">
+        <v>58</v>
+      </c>
+      <c r="P41" t="s">
+        <v>61</v>
+      </c>
+      <c r="S41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" t="s">
+        <v>33</v>
+      </c>
+      <c r="G42">
+        <v>40</v>
+      </c>
+      <c r="J42" t="s">
+        <v>43</v>
+      </c>
+      <c r="K42" t="s">
+        <v>46</v>
+      </c>
+      <c r="L42" t="s">
+        <v>53</v>
+      </c>
+      <c r="M42" t="s">
+        <v>54</v>
+      </c>
+      <c r="O42" t="s">
+        <v>58</v>
+      </c>
+      <c r="P42" t="s">
+        <v>61</v>
+      </c>
+      <c r="S42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43">
+        <v>40</v>
+      </c>
+      <c r="J43" t="s">
+        <v>43</v>
+      </c>
+      <c r="K43" t="s">
+        <v>46</v>
+      </c>
+      <c r="L43" t="s">
+        <v>53</v>
+      </c>
+      <c r="M43" t="s">
+        <v>54</v>
+      </c>
+      <c r="O43" t="s">
+        <v>58</v>
+      </c>
+      <c r="P43" t="s">
+        <v>61</v>
+      </c>
+      <c r="S43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44">
+        <v>40</v>
+      </c>
+      <c r="J44" t="s">
+        <v>43</v>
+      </c>
+      <c r="K44" t="s">
+        <v>46</v>
+      </c>
+      <c r="L44" t="s">
+        <v>53</v>
+      </c>
+      <c r="M44" t="s">
+        <v>54</v>
+      </c>
+      <c r="O44" t="s">
+        <v>58</v>
+      </c>
+      <c r="P44" t="s">
+        <v>61</v>
+      </c>
+      <c r="S44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45">
+        <v>40</v>
+      </c>
+      <c r="J45" t="s">
+        <v>43</v>
+      </c>
+      <c r="K45" t="s">
+        <v>46</v>
+      </c>
+      <c r="L45" t="s">
+        <v>53</v>
+      </c>
+      <c r="M45" t="s">
+        <v>54</v>
+      </c>
+      <c r="O45" t="s">
+        <v>58</v>
+      </c>
+      <c r="P45" t="s">
+        <v>61</v>
+      </c>
+      <c r="S45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" t="s">
+        <v>33</v>
+      </c>
+      <c r="G46">
+        <v>40</v>
+      </c>
+      <c r="J46" t="s">
+        <v>43</v>
+      </c>
+      <c r="K46" t="s">
+        <v>46</v>
+      </c>
+      <c r="L46" t="s">
+        <v>53</v>
+      </c>
+      <c r="M46" t="s">
+        <v>54</v>
+      </c>
+      <c r="O46" t="s">
+        <v>58</v>
+      </c>
+      <c r="P46" t="s">
+        <v>61</v>
+      </c>
+      <c r="S46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+      <c r="G47">
+        <v>35</v>
+      </c>
+      <c r="J47" t="s">
+        <v>43</v>
+      </c>
+      <c r="K47" t="s">
+        <v>46</v>
+      </c>
+      <c r="L47" t="s">
+        <v>53</v>
+      </c>
+      <c r="M47" t="s">
+        <v>54</v>
+      </c>
+      <c r="O47" t="s">
+        <v>58</v>
+      </c>
+      <c r="P47" t="s">
+        <v>61</v>
+      </c>
+      <c r="S47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" t="s">
+        <v>33</v>
+      </c>
+      <c r="G48">
+        <v>35</v>
+      </c>
+      <c r="J48" t="s">
+        <v>43</v>
+      </c>
+      <c r="K48" t="s">
+        <v>46</v>
+      </c>
+      <c r="L48" t="s">
+        <v>53</v>
+      </c>
+      <c r="M48" t="s">
+        <v>54</v>
+      </c>
+      <c r="O48" t="s">
+        <v>58</v>
+      </c>
+      <c r="P48" t="s">
+        <v>61</v>
+      </c>
+      <c r="S48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="S28" t="s">
-        <v>63</v>
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" t="s">
+        <v>33</v>
+      </c>
+      <c r="G49">
+        <v>35</v>
+      </c>
+      <c r="J49" t="s">
+        <v>43</v>
+      </c>
+      <c r="K49" t="s">
+        <v>46</v>
+      </c>
+      <c r="L49" t="s">
+        <v>53</v>
+      </c>
+      <c r="M49" t="s">
+        <v>54</v>
+      </c>
+      <c r="O49" t="s">
+        <v>58</v>
+      </c>
+      <c r="P49" t="s">
+        <v>61</v>
+      </c>
+      <c r="S49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" t="s">
+        <v>33</v>
+      </c>
+      <c r="G50">
+        <v>35</v>
+      </c>
+      <c r="J50" t="s">
+        <v>43</v>
+      </c>
+      <c r="K50" t="s">
+        <v>46</v>
+      </c>
+      <c r="L50" t="s">
+        <v>53</v>
+      </c>
+      <c r="M50" t="s">
+        <v>54</v>
+      </c>
+      <c r="O50" t="s">
+        <v>58</v>
+      </c>
+      <c r="P50" t="s">
+        <v>61</v>
+      </c>
+      <c r="S50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51">
+        <v>35</v>
+      </c>
+      <c r="J51" t="s">
+        <v>43</v>
+      </c>
+      <c r="K51" t="s">
+        <v>46</v>
+      </c>
+      <c r="L51" t="s">
+        <v>53</v>
+      </c>
+      <c r="M51" t="s">
+        <v>54</v>
+      </c>
+      <c r="O51" t="s">
+        <v>58</v>
+      </c>
+      <c r="P51" t="s">
+        <v>61</v>
+      </c>
+      <c r="S51" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" t="s">
+        <v>33</v>
+      </c>
+      <c r="G52">
+        <v>35</v>
+      </c>
+      <c r="J52" t="s">
+        <v>43</v>
+      </c>
+      <c r="K52" t="s">
+        <v>46</v>
+      </c>
+      <c r="L52" t="s">
+        <v>53</v>
+      </c>
+      <c r="M52" t="s">
+        <v>54</v>
+      </c>
+      <c r="O52" t="s">
+        <v>58</v>
+      </c>
+      <c r="P52" t="s">
+        <v>61</v>
+      </c>
+      <c r="S52" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1796,19 +2777,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected the date's method
</commit_message>
<xml_diff>
--- a/appl_register.xlsx
+++ b/appl_register.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="92">
   <si>
     <t>№ Заявки</t>
   </si>
@@ -89,6 +89,9 @@
     <t>самовывоз</t>
   </si>
   <si>
+    <t>автономка доставка</t>
+  </si>
+  <si>
     <t>27.04.2024</t>
   </si>
   <si>
@@ -119,9 +122,15 @@
     <t xml:space="preserve">ЦЕМ I 42.5н Беларусь   </t>
   </si>
   <si>
+    <t xml:space="preserve">ЦЕМ I 42,5н БЦЗ Костюковичи </t>
+  </si>
+  <si>
     <t>Обязательно актуальный паспорт!</t>
   </si>
   <si>
+    <t xml:space="preserve">Машина с пломбами и актуальными паспортами </t>
+  </si>
+  <si>
     <t>куб</t>
   </si>
   <si>
@@ -161,6 +170,9 @@
     <t>псо 13</t>
   </si>
   <si>
+    <t xml:space="preserve">СЗТК </t>
+  </si>
+  <si>
     <t>АО "МСУ-1"</t>
   </si>
   <si>
@@ -179,6 +191,9 @@
     <t xml:space="preserve">ООО ""ТД"Цемент </t>
   </si>
   <si>
+    <t>ООО "КАНТАН"</t>
+  </si>
+  <si>
     <t>ООО "ТД"Цемент</t>
   </si>
   <si>
@@ -203,9 +218,15 @@
     <t>+7 910 404-06-14</t>
   </si>
   <si>
+    <t>+79777728931</t>
+  </si>
+  <si>
     <t>с 9.00 до 20.00</t>
   </si>
   <si>
+    <t>к 9</t>
+  </si>
+  <si>
     <t>оплата 250</t>
   </si>
   <si>
@@ -252,6 +273,18 @@
   </si>
   <si>
     <t xml:space="preserve"> ИГО:  Заявка на доставку  1. Дата отгрузки 28.04.2023  2. Марка ЦЕМ I 42.5н Беларусь    3. Количество тонн: 200   4. От ООО Спарта  5. Завод: Сзтк  6. Покупатель ООО ""ТД"Цемент  7. Грузополучатель: ООО "ТД"Цемент   8. Голицыно +7 910 404-06-14 РБУ Можайское ш., 81 </t>
+  </si>
+  <si>
+    <t>\nЮра Менеджер:\nЗаявка на доставку (автономка) \n1. Дата отгрузки: 28.04.24 \n2. Марка: ЦЕМ I 42,5н БЦЗ Костюковичи \nМашина с пломбами и актуальными паспортами \n3. Количество: 40т.\n4. Продажа от: ООО "Спарта"\n5. Перевалка: СЗТК \n6. Покупатель: ООО "КАНТАН"\n7. Грузополучатель: ООО "КАНТАН"\n8. Время приёмки: к 9 \n9. Контакт диспетчера: +79777728931 \n10. Точка выгрузки: территориальное управление Соколовское\nгородской округ Солнечногорск, Московская область\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Юра Менеджер: Заявка на доставку (автономка)  1. Дата отгрузки: 28.04  2. Марка: ЦЕМ I 42,5н БЦЗ Костюковичи  Машина с пломбами и актуальными паспортами  3. Количество: 40т. 4. Продажа от: ООО "Спарта" 5. Перевалка: СЗТК  6. Покупатель: ООО "КАНТАН" 7. Грузополучатель: ООО "КАНТАН" 8. Время приёмки: к 9  9. Контакт диспетчера: +79777728931  10. Точка выгрузки: территориальное управление Соколовское городской округ Солнечногорск, Московская область </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Юра Менеджер: Заявка на доставку (автономка)  1. Дата отгрузки: 28.04.24  2. Марка: ЦЕМ I 42,5н БЦЗ Костюковичи  Машина с пломбами и актуальными паспортами  3. Количество: 40т. 4. Продажа от: ООО "Спарта" 5. Перевалка: СЗТК  6. Покупатель: ООО "КАНТАН" 7. Грузополучатель: ООО "КАНТАН" 8. Время приёмки: к 9  9. Контакт диспетчера: +79777728931  10. Точка выгрузки: территориальное управление Соколовское городской округ Солнечногорск, Московская область </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Юра Менеджер: Заявка на доставку (автономка)  1. Дата отгрузки: 28.04.23  2. Марка: ЦЕМ I 42,5н БЦЗ Костюковичи  Машина с пломбами и актуальными паспортами  3. Количество: 40т. 4. Продажа от: ООО "Спарта" 5. Перевалка: СЗТК  6. Покупатель: ООО "КАНТАН" 7. Грузополучатель: ООО "КАНТАН" 8. Время приёмки: к 9  9. Контакт диспетчера: +79777728931  10. Точка выгрузки: территориальное управление Соколовское городской округ Солнечногорск, Московская область </t>
   </si>
   <si>
     <t>Ошибка</t>
@@ -622,13 +655,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S52"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -700,40 +736,40 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2">
         <v>200</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -747,40 +783,40 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G3">
         <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="P3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="R3" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="S3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
@@ -794,40 +830,40 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4">
         <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="R4" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="S4" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -841,40 +877,40 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5">
         <v>80</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="P5" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="R5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="S5" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
@@ -888,40 +924,40 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <v>80</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="R6" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="S6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
@@ -935,40 +971,40 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="P7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="R7" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="S7" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
@@ -982,40 +1018,40 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="P8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="R8" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="S8" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
@@ -1029,40 +1065,40 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G9">
         <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="P9" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="R9" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="S9" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -1076,40 +1112,40 @@
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G10">
         <v>40</v>
       </c>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P10" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="Q10" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S10" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -1123,40 +1159,40 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G11">
         <v>40</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O11" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P11" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="Q11" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
@@ -1170,40 +1206,40 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G12">
         <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O12" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P12" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="Q12" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S12" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -1217,40 +1253,40 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G13">
         <v>40</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K13" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O13" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P13" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="Q13" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S13" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -1264,40 +1300,40 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G14">
         <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J14" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O14" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P14" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="Q14" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S14" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
@@ -1311,40 +1347,40 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G15">
         <v>40</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O15" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P15" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="Q15" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S15" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
@@ -1358,40 +1394,40 @@
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G16">
         <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J16" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K16" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O16" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P16" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="Q16" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S16" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
@@ -1405,40 +1441,40 @@
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G17">
         <v>40</v>
       </c>
       <c r="H17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J17" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L17" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M17" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O17" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P17" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="Q17" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S17" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
@@ -1452,40 +1488,40 @@
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G18">
         <v>40</v>
       </c>
       <c r="H18" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J18" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K18" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L18" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M18" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O18" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="Q18" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S18" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
@@ -1499,40 +1535,40 @@
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G19">
         <v>40</v>
       </c>
       <c r="H19" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J19" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K19" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L19" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M19" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O19" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P19" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="Q19" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="S19" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
@@ -1540,7 +1576,7 @@
         <v>19</v>
       </c>
       <c r="S20" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
@@ -1551,31 +1587,31 @@
         <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G21">
         <v>40</v>
       </c>
       <c r="H21" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I21" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J21" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L21" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="S21" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
@@ -1586,31 +1622,31 @@
         <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G22">
         <v>40</v>
       </c>
       <c r="H22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I22" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L22" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="S22" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
@@ -1621,31 +1657,31 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G23">
         <v>40</v>
       </c>
       <c r="H23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I23" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J23" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K23" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L23" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="S23" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
@@ -1659,34 +1695,34 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G24">
         <v>40</v>
       </c>
       <c r="H24" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K24" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L24" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="M24" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="O24" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="S24" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
@@ -1700,34 +1736,34 @@
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G25">
         <v>40</v>
       </c>
       <c r="H25" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J25" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K25" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L25" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="M25" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="O25" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="S25" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
@@ -1741,31 +1777,31 @@
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F26" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G26">
         <v>40</v>
       </c>
       <c r="H26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I26" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J26" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="L26" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="S26" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
@@ -1779,31 +1815,31 @@
         <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G27">
         <v>40</v>
       </c>
       <c r="H27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I27" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J27" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="L27" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="S27" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
@@ -1817,31 +1853,31 @@
         <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G28">
         <v>40</v>
       </c>
       <c r="H28" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I28" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J28" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="L28" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="S28" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
@@ -1849,7 +1885,7 @@
         <v>28</v>
       </c>
       <c r="S29" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
@@ -1860,31 +1896,31 @@
         <v>23</v>
       </c>
       <c r="D30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G30">
         <v>35</v>
       </c>
       <c r="H30" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I30" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J30" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K30" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L30" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="S30" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
@@ -1895,31 +1931,31 @@
         <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G31">
         <v>35</v>
       </c>
       <c r="H31" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I31" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J31" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K31" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L31" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="S31" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
@@ -1933,37 +1969,37 @@
         <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G32">
         <v>35</v>
       </c>
       <c r="H32" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J32" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K32" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L32" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M32" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O32" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P32" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S32" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
@@ -1977,34 +2013,34 @@
         <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G33">
         <v>40</v>
       </c>
       <c r="J33" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K33" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L33" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M33" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O33" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P33" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S33" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.35">
@@ -2018,34 +2054,34 @@
         <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G34">
         <v>40</v>
       </c>
       <c r="J34" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K34" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L34" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M34" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O34" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P34" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S34" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.35">
@@ -2059,34 +2095,34 @@
         <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G35">
         <v>40</v>
       </c>
       <c r="J35" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K35" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L35" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M35" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O35" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P35" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S35" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
@@ -2100,34 +2136,34 @@
         <v>22</v>
       </c>
       <c r="D36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E36" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G36">
         <v>40</v>
       </c>
       <c r="J36" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K36" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L36" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M36" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O36" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P36" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S36" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.35">
@@ -2141,34 +2177,34 @@
         <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G37">
         <v>40</v>
       </c>
       <c r="J37" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K37" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L37" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M37" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O37" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P37" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S37" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.35">
@@ -2182,34 +2218,34 @@
         <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E38" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G38">
         <v>40</v>
       </c>
       <c r="J38" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K38" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L38" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M38" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O38" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P38" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S38" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.35">
@@ -2223,34 +2259,34 @@
         <v>22</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E39" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G39">
         <v>40</v>
       </c>
       <c r="J39" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K39" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L39" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M39" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O39" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P39" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S39" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
@@ -2264,34 +2300,34 @@
         <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G40">
         <v>40</v>
       </c>
       <c r="J40" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K40" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L40" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M40" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O40" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P40" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S40" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.35">
@@ -2305,34 +2341,34 @@
         <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G41">
         <v>40</v>
       </c>
       <c r="J41" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L41" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M41" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O41" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P41" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S41" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.35">
@@ -2343,34 +2379,34 @@
         <v>22</v>
       </c>
       <c r="D42" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E42" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G42">
         <v>40</v>
       </c>
       <c r="J42" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K42" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L42" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M42" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O42" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P42" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S42" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.35">
@@ -2381,34 +2417,34 @@
         <v>22</v>
       </c>
       <c r="D43" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E43" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G43">
         <v>40</v>
       </c>
       <c r="J43" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K43" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L43" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M43" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O43" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P43" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S43" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.35">
@@ -2419,34 +2455,34 @@
         <v>22</v>
       </c>
       <c r="D44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E44" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G44">
         <v>40</v>
       </c>
       <c r="J44" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K44" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L44" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M44" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O44" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P44" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S44" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.35">
@@ -2457,34 +2493,34 @@
         <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G45">
         <v>40</v>
       </c>
       <c r="J45" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K45" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L45" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M45" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O45" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P45" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S45" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.35">
@@ -2495,34 +2531,34 @@
         <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E46" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G46">
         <v>40</v>
       </c>
       <c r="J46" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K46" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L46" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M46" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O46" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P46" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S46" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.35">
@@ -2536,34 +2572,34 @@
         <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G47">
         <v>35</v>
       </c>
       <c r="J47" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K47" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L47" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M47" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O47" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P47" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S47" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.35">
@@ -2577,34 +2613,34 @@
         <v>22</v>
       </c>
       <c r="D48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E48" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G48">
         <v>35</v>
       </c>
       <c r="J48" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K48" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L48" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M48" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O48" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P48" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S48" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.35">
@@ -2618,34 +2654,34 @@
         <v>22</v>
       </c>
       <c r="D49" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E49" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G49">
         <v>35</v>
       </c>
       <c r="J49" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K49" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L49" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M49" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O49" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P49" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S49" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.35">
@@ -2659,34 +2695,34 @@
         <v>22</v>
       </c>
       <c r="D50" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E50" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G50">
         <v>35</v>
       </c>
       <c r="J50" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K50" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L50" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M50" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O50" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P50" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S50" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.35">
@@ -2700,34 +2736,34 @@
         <v>22</v>
       </c>
       <c r="D51" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G51">
         <v>35</v>
       </c>
       <c r="J51" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K51" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L51" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M51" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O51" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P51" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S51" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.35">
@@ -2741,34 +2777,250 @@
         <v>22</v>
       </c>
       <c r="D52" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G52">
         <v>35</v>
       </c>
       <c r="J52" t="s">
+        <v>46</v>
+      </c>
+      <c r="K52" t="s">
+        <v>49</v>
+      </c>
+      <c r="L52" t="s">
+        <v>57</v>
+      </c>
+      <c r="M52" t="s">
+        <v>59</v>
+      </c>
+      <c r="O52" t="s">
+        <v>63</v>
+      </c>
+      <c r="P52" t="s">
+        <v>66</v>
+      </c>
+      <c r="S52" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="S53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" t="s">
+        <v>35</v>
+      </c>
+      <c r="F54" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54">
+        <v>35</v>
+      </c>
+      <c r="H54" t="s">
+        <v>39</v>
+      </c>
+      <c r="J54" t="s">
         <v>43</v>
       </c>
-      <c r="K52" t="s">
-        <v>46</v>
-      </c>
-      <c r="L52" t="s">
-        <v>53</v>
-      </c>
-      <c r="M52" t="s">
+      <c r="K54" t="s">
+        <v>51</v>
+      </c>
+      <c r="L54" t="s">
+        <v>58</v>
+      </c>
+      <c r="M54" t="s">
+        <v>58</v>
+      </c>
+      <c r="O54" t="s">
+        <v>61</v>
+      </c>
+      <c r="P54" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>69</v>
+      </c>
+      <c r="S54" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A55">
         <v>54</v>
       </c>
-      <c r="O52" t="s">
+      <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" t="s">
+        <v>35</v>
+      </c>
+      <c r="F55" t="s">
+        <v>37</v>
+      </c>
+      <c r="G55">
+        <v>35</v>
+      </c>
+      <c r="H55" t="s">
+        <v>39</v>
+      </c>
+      <c r="J55" t="s">
+        <v>43</v>
+      </c>
+      <c r="K55" t="s">
+        <v>51</v>
+      </c>
+      <c r="L55" t="s">
         <v>58</v>
       </c>
-      <c r="P52" t="s">
+      <c r="M55" t="s">
+        <v>58</v>
+      </c>
+      <c r="O55" t="s">
         <v>61</v>
       </c>
-      <c r="S52" t="s">
-        <v>78</v>
+      <c r="P55" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>69</v>
+      </c>
+      <c r="S55" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="S56" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" t="s">
+        <v>37</v>
+      </c>
+      <c r="G57">
+        <v>35</v>
+      </c>
+      <c r="H57" t="s">
+        <v>39</v>
+      </c>
+      <c r="J57" t="s">
+        <v>43</v>
+      </c>
+      <c r="K57" t="s">
+        <v>51</v>
+      </c>
+      <c r="L57" t="s">
+        <v>58</v>
+      </c>
+      <c r="M57" t="s">
+        <v>58</v>
+      </c>
+      <c r="O57" t="s">
+        <v>61</v>
+      </c>
+      <c r="P57" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>69</v>
+      </c>
+      <c r="S57" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" t="s">
+        <v>35</v>
+      </c>
+      <c r="F58" t="s">
+        <v>37</v>
+      </c>
+      <c r="G58">
+        <v>35</v>
+      </c>
+      <c r="H58" t="s">
+        <v>39</v>
+      </c>
+      <c r="J58" t="s">
+        <v>43</v>
+      </c>
+      <c r="K58" t="s">
+        <v>51</v>
+      </c>
+      <c r="L58" t="s">
+        <v>58</v>
+      </c>
+      <c r="M58" t="s">
+        <v>58</v>
+      </c>
+      <c r="O58" t="s">
+        <v>61</v>
+      </c>
+      <c r="P58" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>69</v>
+      </c>
+      <c r="S58" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2786,10 +3038,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>